<commit_message>
Redesigned output to one long page
</commit_message>
<xml_diff>
--- a/db/szperacz.xlsx
+++ b/db/szperacz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projektOrganista\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F899C43-F92A-4742-9230-7F77F6173102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0410133-A134-472E-831F-53D146985F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="2190" windowWidth="14670" windowHeight="8325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="log przeszłości" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2280" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="564">
   <si>
     <t>Data</t>
   </si>
@@ -5698,6 +5698,9 @@
 chwała Ci po wszystkie czasy, miłość, uwielbienie.
 *
 Hosanna, hosanna Synowi Bożemu…</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -5851,7 +5854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5909,6 +5912,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8042,6 +8048,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>115956</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>215349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3379304</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>722465</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Obraz 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0BFD307-5606-2D8D-2626-65CA20F5BA30}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="115956" y="6170545"/>
+          <a:ext cx="3263348" cy="507116"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -13310,8 +13360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA72C7D-2EFC-408F-B255-EAEC24F0A3D2}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13468,27 +13518,29 @@
       <c r="A11" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="12" t="s">
         <v>228</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="27" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="B12" s="27"/>
       <c r="C12" s="12" t="s">
         <v>225</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="E12" s="26"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" spans="1:5" s="19" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -13509,30 +13561,30 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="27" t="s">
         <v>222</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="27" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="3:3" s="19" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
@@ -13556,8 +13608,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A11:A12"/>
+  <mergeCells count="6">
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="A15:A16"/>
@@ -13577,7 +13628,7 @@
   </sheetPr>
   <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
Fixed exit button's position in song adder
</commit_message>
<xml_diff>
--- a/db/szperacz.xlsx
+++ b/db/szperacz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projektOrganista\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0410133-A134-472E-831F-53D146985F24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2150D94C-10D2-435E-A86E-73AB62A2CEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8250" yWindow="1830" windowWidth="20910" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="log przeszłości" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2281" uniqueCount="565">
   <si>
     <t>Data</t>
   </si>
@@ -5701,6 +5701,9 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>0/1/0/1/1/0</t>
   </si>
 </sst>
 </file>
@@ -13360,7 +13363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA72C7D-2EFC-408F-B255-EAEC24F0A3D2}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -13623,16 +13626,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F891C4F-9816-403C-B080-E89BC2162DC9}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="A1:G200"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G201" sqref="G201"/>
+      <selection pane="bottomRight" activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13668,7 +13671,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -13714,7 +13717,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -13737,7 +13740,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>241</v>
       </c>
@@ -13760,7 +13763,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -13780,7 +13783,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>104</v>
       </c>
@@ -13803,7 +13806,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -13826,7 +13829,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>207</v>
       </c>
@@ -13849,7 +13852,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -13872,7 +13875,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -13895,7 +13898,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>143</v>
       </c>
@@ -13918,7 +13921,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>202</v>
       </c>
@@ -13941,7 +13944,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -13964,7 +13967,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>194</v>
       </c>
@@ -13987,7 +13990,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>144</v>
       </c>
@@ -14010,7 +14013,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>147</v>
       </c>
@@ -14033,7 +14036,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -14056,7 +14059,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -14079,7 +14082,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -14102,7 +14105,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>148</v>
       </c>
@@ -14125,7 +14128,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>149</v>
       </c>
@@ -14148,7 +14151,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>242</v>
       </c>
@@ -14171,7 +14174,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -14194,7 +14197,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -14217,7 +14220,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -14240,7 +14243,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>320</v>
       </c>
@@ -14263,7 +14266,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>150</v>
       </c>
@@ -14286,7 +14289,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -14309,7 +14312,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>199</v>
       </c>
@@ -14332,7 +14335,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>151</v>
       </c>
@@ -14355,7 +14358,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>152</v>
       </c>
@@ -14378,7 +14381,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -14401,7 +14404,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -14424,7 +14427,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>323</v>
       </c>
@@ -14441,7 +14444,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -14464,7 +14467,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -14487,7 +14490,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -14510,7 +14513,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>321</v>
       </c>
@@ -14530,7 +14533,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -14553,7 +14556,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -14570,13 +14573,13 @@
         <v>173</v>
       </c>
       <c r="F41" t="s">
-        <v>340</v>
+        <v>564</v>
       </c>
       <c r="G41" s="25" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -14599,7 +14602,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>102</v>
       </c>
@@ -14622,7 +14625,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -14645,7 +14648,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>16</v>
       </c>
@@ -14668,7 +14671,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>376</v>
       </c>
@@ -14688,7 +14691,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>110</v>
       </c>
@@ -14711,7 +14714,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -14757,7 +14760,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>91</v>
       </c>
@@ -14777,7 +14780,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>30</v>
       </c>
@@ -14800,7 +14803,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -14823,7 +14826,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -14846,7 +14849,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>153</v>
       </c>
@@ -14869,7 +14872,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>111</v>
       </c>
@@ -14892,7 +14895,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>273</v>
       </c>
@@ -14912,7 +14915,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -14935,7 +14938,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>112</v>
       </c>
@@ -14958,7 +14961,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>113</v>
       </c>
@@ -14981,7 +14984,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>32</v>
       </c>
@@ -15004,7 +15007,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>33</v>
       </c>
@@ -15027,7 +15030,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -15073,7 +15076,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>243</v>
       </c>
@@ -15116,7 +15119,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>35</v>
       </c>
@@ -15139,7 +15142,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>36</v>
       </c>
@@ -15162,7 +15165,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>37</v>
       </c>
@@ -15185,7 +15188,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>154</v>
       </c>
@@ -15202,13 +15205,13 @@
         <v>179</v>
       </c>
       <c r="F69" t="s">
-        <v>336</v>
+        <v>362</v>
       </c>
       <c r="G69" s="25" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -15231,7 +15234,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>155</v>
       </c>
@@ -15254,7 +15257,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -15277,7 +15280,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>40</v>
       </c>
@@ -15323,7 +15326,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>156</v>
       </c>
@@ -15346,7 +15349,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>157</v>
       </c>
@@ -15369,7 +15372,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>41</v>
       </c>
@@ -15392,7 +15395,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>44</v>
       </c>
@@ -15415,7 +15418,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>114</v>
       </c>
@@ -15438,7 +15441,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -15461,7 +15464,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>43</v>
       </c>
@@ -15484,7 +15487,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>190</v>
       </c>
@@ -15507,7 +15510,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>45</v>
       </c>
@@ -15530,7 +15533,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>46</v>
       </c>
@@ -15553,7 +15556,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>94</v>
       </c>
@@ -15576,7 +15579,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>208</v>
       </c>
@@ -15599,7 +15602,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>47</v>
       </c>
@@ -15622,7 +15625,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -15645,7 +15648,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>49</v>
       </c>
@@ -15668,7 +15671,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>50</v>
       </c>
@@ -15691,7 +15694,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>51</v>
       </c>
@@ -15737,7 +15740,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>52</v>
       </c>
@@ -15760,7 +15763,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>130</v>
       </c>
@@ -15806,7 +15809,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>115</v>
       </c>
@@ -15829,7 +15832,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>53</v>
       </c>
@@ -15852,7 +15855,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>54</v>
       </c>
@@ -15875,7 +15878,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>116</v>
       </c>
@@ -15898,7 +15901,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>55</v>
       </c>
@@ -15921,7 +15924,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>117</v>
       </c>
@@ -15944,7 +15947,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>56</v>
       </c>
@@ -15967,7 +15970,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>57</v>
       </c>
@@ -15990,7 +15993,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>274</v>
       </c>
@@ -16013,7 +16016,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>158</v>
       </c>
@@ -16036,7 +16039,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>244</v>
       </c>
@@ -16059,7 +16062,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>210</v>
       </c>
@@ -16082,7 +16085,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>247</v>
       </c>
@@ -16105,7 +16108,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>60</v>
       </c>
@@ -16128,7 +16131,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>138</v>
       </c>
@@ -16148,7 +16151,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>58</v>
       </c>
@@ -16171,7 +16174,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>262</v>
       </c>
@@ -16194,7 +16197,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>137</v>
       </c>
@@ -16214,7 +16217,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>381</v>
       </c>
@@ -16237,7 +16240,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>59</v>
       </c>
@@ -16260,7 +16263,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>118</v>
       </c>
@@ -16283,7 +16286,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>61</v>
       </c>
@@ -16306,7 +16309,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>240</v>
       </c>
@@ -16352,7 +16355,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>160</v>
       </c>
@@ -16375,7 +16378,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>63</v>
       </c>
@@ -16398,7 +16401,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>64</v>
       </c>
@@ -16421,7 +16424,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>15</v>
       </c>
@@ -16444,7 +16447,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>95</v>
       </c>
@@ -16490,7 +16493,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>62</v>
       </c>
@@ -16513,7 +16516,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>103</v>
       </c>
@@ -16536,7 +16539,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>204</v>
       </c>
@@ -16559,7 +16562,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>139</v>
       </c>
@@ -16579,7 +16582,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>236</v>
       </c>
@@ -16602,7 +16605,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>65</v>
       </c>
@@ -16625,7 +16628,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>66</v>
       </c>
@@ -16648,7 +16651,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>246</v>
       </c>
@@ -16671,7 +16674,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>10</v>
       </c>
@@ -16694,7 +16697,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>67</v>
       </c>
@@ -16717,7 +16720,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>69</v>
       </c>
@@ -16740,7 +16743,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>237</v>
       </c>
@@ -16763,7 +16766,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>68</v>
       </c>
@@ -16786,7 +16789,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>13</v>
       </c>
@@ -16809,7 +16812,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>380</v>
       </c>
@@ -16832,7 +16835,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>334</v>
       </c>
@@ -16875,7 +16878,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>70</v>
       </c>
@@ -16898,7 +16901,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>161</v>
       </c>
@@ -16921,7 +16924,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>119</v>
       </c>
@@ -16944,7 +16947,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>96</v>
       </c>
@@ -16967,7 +16970,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>97</v>
       </c>
@@ -16990,7 +16993,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>120</v>
       </c>
@@ -17013,7 +17016,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>71</v>
       </c>
@@ -17036,7 +17039,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>193</v>
       </c>
@@ -17059,7 +17062,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>162</v>
       </c>
@@ -17082,7 +17085,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>72</v>
       </c>
@@ -17128,7 +17131,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>265</v>
       </c>
@@ -17151,7 +17154,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>188</v>
       </c>
@@ -17174,7 +17177,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>163</v>
       </c>
@@ -17197,7 +17200,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>74</v>
       </c>
@@ -17220,7 +17223,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>75</v>
       </c>
@@ -17243,7 +17246,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>164</v>
       </c>
@@ -17266,7 +17269,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>76</v>
       </c>
@@ -17289,7 +17292,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>77</v>
       </c>
@@ -17312,7 +17315,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>305</v>
       </c>
@@ -17335,7 +17338,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>98</v>
       </c>
@@ -17358,7 +17361,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>121</v>
       </c>
@@ -17381,7 +17384,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>78</v>
       </c>
@@ -17404,7 +17407,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>99</v>
       </c>
@@ -17427,7 +17430,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>79</v>
       </c>
@@ -17450,7 +17453,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>186</v>
       </c>
@@ -17473,7 +17476,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>165</v>
       </c>
@@ -17496,7 +17499,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>80</v>
       </c>
@@ -17519,7 +17522,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>122</v>
       </c>
@@ -17565,7 +17568,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>125</v>
       </c>
@@ -17588,7 +17591,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>140</v>
       </c>
@@ -17608,7 +17611,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>123</v>
       </c>
@@ -17631,7 +17634,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>141</v>
       </c>
@@ -17651,7 +17654,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>81</v>
       </c>
@@ -17697,7 +17700,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>205</v>
       </c>
@@ -17720,7 +17723,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>166</v>
       </c>
@@ -17743,7 +17746,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>82</v>
       </c>
@@ -17766,7 +17769,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>83</v>
       </c>
@@ -17812,7 +17815,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>272</v>
       </c>
@@ -17832,7 +17835,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>84</v>
       </c>
@@ -17855,7 +17858,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>9</v>
       </c>
@@ -17878,7 +17881,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>124</v>
       </c>
@@ -17901,7 +17904,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>86</v>
       </c>
@@ -17924,7 +17927,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>126</v>
       </c>
@@ -17947,7 +17950,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>169</v>
       </c>
@@ -17970,7 +17973,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>167</v>
       </c>
@@ -17993,7 +17996,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>192</v>
       </c>
@@ -18016,7 +18019,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>100</v>
       </c>
@@ -18039,7 +18042,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>101</v>
       </c>
@@ -18062,7 +18065,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>85</v>
       </c>
@@ -18085,7 +18088,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>87</v>
       </c>
@@ -18108,7 +18111,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>12</v>
       </c>
@@ -18131,7 +18134,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>168</v>
       </c>
@@ -18154,7 +18157,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>170</v>
       </c>
@@ -18177,7 +18180,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>142</v>
       </c>
@@ -18198,13 +18201,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G200" xr:uid="{4F891C4F-9816-403C-B080-E89BC2162DC9}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="7"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G200" xr:uid="{4F891C4F-9816-403C-B080-E89BC2162DC9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Repaired underlining in lyrics
</commit_message>
<xml_diff>
--- a/db/szperacz.xlsx
+++ b/db/szperacz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projektOrganista\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2150D94C-10D2-435E-A86E-73AB62A2CEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569977A0-A124-45C7-ACA5-771890C19F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8250" yWindow="1830" windowWidth="20910" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="1830" windowWidth="20910" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="log przeszłości" sheetId="1" r:id="rId1"/>
@@ -3106,32 +3106,6 @@
   </si>
   <si>
     <t>*
-Jam jest chlebem żywym
-Który zstąpił z nieba
-**
-1.
-Ciało moje _est pokarmem
-A krew mo_ja_ jest napojem
-*
-Jam jest chlebem żywym…
-2.
-Kto pożywa Ciało i Krew moją
-Ten _ma_ życie wieczne
-*
-Jam jest chlebem żywym…
-3.
-Kto przyjmuje Ciało i Krew moją
-Ten we Mnie, _a_ Ja w nim mieszkam
-*
-Jam jest chlebem żywym…
-4.
-Ja go wskrzeszę w dzień ostateczny
-I bę_dzie_ żył na wieki
-*
-Jam jest chlebem żywym…</t>
-  </si>
-  <si>
-    <t>*
 Jasnogórska Pani, Tyś naszą hetmanką
 Polski Tyś Królową i najlepszą Matką
 **
@@ -5704,6 +5678,32 @@
   </si>
   <si>
     <t>0/1/0/1/1/0</t>
+  </si>
+  <si>
+    <t>*
+Jam jest chlebem żywym
+Który zstąpił z nieba
+**
+1.
+Ciało moje _jest_ pokarmem
+A krew mo_ja_ jest napojem
+*
+Jam jest chlebem żywym…
+2.
+Kto pożywa Ciało i Krew moją
+Ten _ma_ życie wieczne
+*
+Jam jest chlebem żywym…
+3.
+Kto przyjmuje Ciało i Krew moją
+Ten we Mnie, _a_ Ja w nim mieszkam
+*
+Jam jest chlebem żywym…
+4.
+Ja go wskrzeszę w dzień ostateczny
+I bę_dzie_ żył na wieki
+*
+Jam jest chlebem żywym…</t>
   </si>
 </sst>
 </file>
@@ -13534,7 +13534,7 @@
     </row>
     <row r="12" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="12" t="s">
@@ -13632,10 +13632,10 @@
   <dimension ref="A1:G200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F71" sqref="F71"/>
+      <selection pane="bottomRight" activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -13714,7 +13714,7 @@
         <v>336</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13737,7 +13737,7 @@
         <v>335</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13760,7 +13760,7 @@
         <v>335</v>
       </c>
       <c r="G5" s="25" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13803,7 +13803,7 @@
         <v>335</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13826,7 +13826,7 @@
         <v>337</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -13987,7 +13987,7 @@
         <v>344</v>
       </c>
       <c r="G15" s="25" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14194,7 +14194,7 @@
         <v>335</v>
       </c>
       <c r="G24" s="25" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14217,7 +14217,7 @@
         <v>335</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14464,7 +14464,7 @@
         <v>335</v>
       </c>
       <c r="G36" s="25" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14573,7 +14573,7 @@
         <v>173</v>
       </c>
       <c r="F41" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G41" s="25" t="s">
         <v>435</v>
@@ -14622,7 +14622,7 @@
         <v>344</v>
       </c>
       <c r="G43" s="25" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14711,7 +14711,7 @@
         <v>335</v>
       </c>
       <c r="G47" s="25" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14757,7 +14757,7 @@
         <v>335</v>
       </c>
       <c r="G49" s="25" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14892,7 +14892,7 @@
         <v>335</v>
       </c>
       <c r="G55" s="25" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14958,7 +14958,7 @@
         <v>335</v>
       </c>
       <c r="G58" s="25" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -14981,7 +14981,7 @@
         <v>335</v>
       </c>
       <c r="G59" s="25" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15073,7 +15073,7 @@
         <v>341</v>
       </c>
       <c r="G63" s="25" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15096,7 +15096,7 @@
         <v>335</v>
       </c>
       <c r="G64" s="25" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15254,7 +15254,7 @@
         <v>341</v>
       </c>
       <c r="G71" s="25" t="s">
-        <v>450</v>
+        <v>564</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15277,7 +15277,7 @@
         <v>347</v>
       </c>
       <c r="G72" s="25" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15300,7 +15300,7 @@
         <v>341</v>
       </c>
       <c r="G73" s="25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15323,7 +15323,7 @@
         <v>362</v>
       </c>
       <c r="G74" s="25" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15346,7 +15346,7 @@
         <v>341</v>
       </c>
       <c r="G75" s="25" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15369,7 +15369,7 @@
         <v>341</v>
       </c>
       <c r="G76" s="25" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15392,7 +15392,7 @@
         <v>360</v>
       </c>
       <c r="G77" s="25" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15415,7 +15415,7 @@
         <v>341</v>
       </c>
       <c r="G78" s="25" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15438,7 +15438,7 @@
         <v>335</v>
       </c>
       <c r="G79" s="25" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15461,7 +15461,7 @@
         <v>341</v>
       </c>
       <c r="G80" s="25" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15484,7 +15484,7 @@
         <v>341</v>
       </c>
       <c r="G81" s="25" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15507,7 +15507,7 @@
         <v>354</v>
       </c>
       <c r="G82" s="25" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15530,7 +15530,7 @@
         <v>354</v>
       </c>
       <c r="G83" s="25" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15553,7 +15553,7 @@
         <v>342</v>
       </c>
       <c r="G84" s="25" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15599,7 +15599,7 @@
         <v>341</v>
       </c>
       <c r="G86" s="25" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15622,7 +15622,7 @@
         <v>341</v>
       </c>
       <c r="G87" s="25" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15645,7 +15645,7 @@
         <v>362</v>
       </c>
       <c r="G88" s="25" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15668,7 +15668,7 @@
         <v>343</v>
       </c>
       <c r="G89" s="25" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15691,7 +15691,7 @@
         <v>355</v>
       </c>
       <c r="G90" s="25" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15714,7 +15714,7 @@
         <v>347</v>
       </c>
       <c r="G91" s="25" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15737,7 +15737,7 @@
         <v>342</v>
       </c>
       <c r="G92" s="25" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15760,7 +15760,7 @@
         <v>336</v>
       </c>
       <c r="G93" s="25" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15806,7 +15806,7 @@
         <v>341</v>
       </c>
       <c r="G95" s="25" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15829,7 +15829,7 @@
         <v>335</v>
       </c>
       <c r="G96" s="25" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15852,7 +15852,7 @@
         <v>342</v>
       </c>
       <c r="G97" s="25" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15875,7 +15875,7 @@
         <v>347</v>
       </c>
       <c r="G98" s="25" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15898,7 +15898,7 @@
         <v>335</v>
       </c>
       <c r="G99" s="25" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15921,7 +15921,7 @@
         <v>342</v>
       </c>
       <c r="G100" s="25" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15944,7 +15944,7 @@
         <v>335</v>
       </c>
       <c r="G101" s="25" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15967,7 +15967,7 @@
         <v>347</v>
       </c>
       <c r="G102" s="25" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -15990,7 +15990,7 @@
         <v>347</v>
       </c>
       <c r="G103" s="25" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16036,7 +16036,7 @@
         <v>363</v>
       </c>
       <c r="G105" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16059,7 +16059,7 @@
         <v>335</v>
       </c>
       <c r="G106" s="25" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16082,7 +16082,7 @@
         <v>341</v>
       </c>
       <c r="G107" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16105,7 +16105,7 @@
         <v>347</v>
       </c>
       <c r="G108" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16171,7 +16171,7 @@
         <v>337</v>
       </c>
       <c r="G111" s="25" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16194,7 +16194,7 @@
         <v>350</v>
       </c>
       <c r="G112" s="25" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16260,7 +16260,7 @@
         <v>346</v>
       </c>
       <c r="G115" s="25" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16283,7 +16283,7 @@
         <v>335</v>
       </c>
       <c r="G116" s="25" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16306,7 +16306,7 @@
         <v>365</v>
       </c>
       <c r="G117" s="25" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16329,7 +16329,7 @@
         <v>335</v>
       </c>
       <c r="G118" s="25" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16352,7 +16352,7 @@
         <v>341</v>
       </c>
       <c r="G119" s="25" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16375,7 +16375,7 @@
         <v>341</v>
       </c>
       <c r="G120" s="25" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16398,7 +16398,7 @@
         <v>341</v>
       </c>
       <c r="G121" s="25" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16421,7 +16421,7 @@
         <v>349</v>
       </c>
       <c r="G122" s="25" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16444,7 +16444,7 @@
         <v>366</v>
       </c>
       <c r="G123" s="25" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16490,7 +16490,7 @@
         <v>355</v>
       </c>
       <c r="G125" s="25" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16513,7 +16513,7 @@
         <v>341</v>
       </c>
       <c r="G126" s="25" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16536,7 +16536,7 @@
         <v>367</v>
       </c>
       <c r="G127" s="25" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16602,7 +16602,7 @@
         <v>342</v>
       </c>
       <c r="G130" s="25" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16625,7 +16625,7 @@
         <v>341</v>
       </c>
       <c r="G131" s="25" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16648,7 +16648,7 @@
         <v>341</v>
       </c>
       <c r="G132" s="25" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16671,7 +16671,7 @@
         <v>341</v>
       </c>
       <c r="G133" s="25" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16694,7 +16694,7 @@
         <v>360</v>
       </c>
       <c r="G134" s="25" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16740,7 +16740,7 @@
         <v>355</v>
       </c>
       <c r="G136" s="25" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16763,7 +16763,7 @@
         <v>368</v>
       </c>
       <c r="G137" s="25" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16786,7 +16786,7 @@
         <v>347</v>
       </c>
       <c r="G138" s="25" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16809,7 +16809,7 @@
         <v>352</v>
       </c>
       <c r="G139" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16875,7 +16875,7 @@
         <v>369</v>
       </c>
       <c r="G142" s="25" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16921,7 +16921,7 @@
         <v>336</v>
       </c>
       <c r="G144" s="25" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -16944,7 +16944,7 @@
         <v>335</v>
       </c>
       <c r="G145" s="25" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17013,7 +17013,7 @@
         <v>335</v>
       </c>
       <c r="G148" s="25" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17036,7 +17036,7 @@
         <v>342</v>
       </c>
       <c r="G149" s="25" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17082,7 +17082,7 @@
         <v>342</v>
       </c>
       <c r="G151" s="25" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17105,7 +17105,7 @@
         <v>354</v>
       </c>
       <c r="G152" s="25" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17128,7 +17128,7 @@
         <v>349</v>
       </c>
       <c r="G153" s="25" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17151,7 +17151,7 @@
         <v>341</v>
       </c>
       <c r="G154" s="25" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17174,7 +17174,7 @@
         <v>341</v>
       </c>
       <c r="G155" s="25" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17197,7 +17197,7 @@
         <v>342</v>
       </c>
       <c r="G156" s="25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17220,7 +17220,7 @@
         <v>347</v>
       </c>
       <c r="G157" s="25" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17243,7 +17243,7 @@
         <v>347</v>
       </c>
       <c r="G158" s="25" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17312,7 +17312,7 @@
         <v>337</v>
       </c>
       <c r="G161" s="25" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17381,7 +17381,7 @@
         <v>335</v>
       </c>
       <c r="G164" s="25" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17404,7 +17404,7 @@
         <v>365</v>
       </c>
       <c r="G165" s="25" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17450,7 +17450,7 @@
         <v>341</v>
       </c>
       <c r="G167" s="25" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17473,7 +17473,7 @@
         <v>349</v>
       </c>
       <c r="G168" s="25" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17496,7 +17496,7 @@
         <v>350</v>
       </c>
       <c r="G169" s="25" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17542,7 +17542,7 @@
         <v>335</v>
       </c>
       <c r="G171" s="25" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17565,7 +17565,7 @@
         <v>347</v>
       </c>
       <c r="G172" s="25" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17588,7 +17588,7 @@
         <v>335</v>
       </c>
       <c r="G173" s="25" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17631,7 +17631,7 @@
         <v>335</v>
       </c>
       <c r="G175" s="25" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17674,7 +17674,7 @@
         <v>350</v>
       </c>
       <c r="G177" s="25" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17697,7 +17697,7 @@
         <v>341</v>
       </c>
       <c r="G178" s="25" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17720,7 +17720,7 @@
         <v>341</v>
       </c>
       <c r="G179" s="25" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17789,7 +17789,7 @@
         <v>336</v>
       </c>
       <c r="G182" s="25" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17812,7 +17812,7 @@
         <v>373</v>
       </c>
       <c r="G183" s="25" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17878,7 +17878,7 @@
         <v>359</v>
       </c>
       <c r="G186" s="25" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17901,7 +17901,7 @@
         <v>335</v>
       </c>
       <c r="G187" s="25" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17924,7 +17924,7 @@
         <v>347</v>
       </c>
       <c r="G188" s="25" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17947,7 +17947,7 @@
         <v>335</v>
       </c>
       <c r="G189" s="25" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -17993,7 +17993,7 @@
         <v>342</v>
       </c>
       <c r="G191" s="25" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -18085,7 +18085,7 @@
         <v>341</v>
       </c>
       <c r="G195" s="25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -18108,7 +18108,7 @@
         <v>337</v>
       </c>
       <c r="G196" s="25" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="197" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -18131,7 +18131,7 @@
         <v>342</v>
       </c>
       <c r="G197" s="25" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="198" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -18154,7 +18154,7 @@
         <v>343</v>
       </c>
       <c r="G198" s="25" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="199" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -18177,7 +18177,7 @@
         <v>341</v>
       </c>
       <c r="G199" s="25" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New songs and new fixed parts
</commit_message>
<xml_diff>
--- a/db/szperacz.xlsx
+++ b/db/szperacz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\projektOrganista\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E099CC1F-5EC4-4212-A4C3-44CB43AB413E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6549DC-8DDA-4CC2-9003-0E82FFAB8461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="log przeszłości" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="side view" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">db!$A$1:$G$203</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">db!$A$1:$G$209</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'lista pieśni'!$A$1:$K$197</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="585">
   <si>
     <t>Data</t>
   </si>
@@ -5791,6 +5791,108 @@
   </si>
   <si>
     <t>Abba Ojcze</t>
+  </si>
+  <si>
+    <t>Miłość Twa</t>
+  </si>
+  <si>
+    <t>1/1/1/1/1/ślubne</t>
+  </si>
+  <si>
+    <t>Miłość Twa
+od najwyższych gór wyższa jest,
+Wielka jest wierność Twa
+Do nieba sięga wzwyż
+Miłość Twa
+głębsza niż ocean bez dna
+wielka jest wierność Twa
+gdy do mnie zbliżasz się.</t>
+  </si>
+  <si>
+    <t>Kiedy serca dwa</t>
+  </si>
+  <si>
+    <t>Kiedy serca dwa połączą się miłością.
+A Bóg obdarzył je łaską Swą
+Wtedy razem iść przez życie chcą z ufnością
+i proszą, żebyś błogosławił im.
+Dziś spójrz, stoją tu u Twoich drzwi
+i proszą, byś zawsze z nimi był.
+Dziś spójrz, stoją tu i proszą Cię,
+byś błogosławił im przez wszystkie dni.</t>
+  </si>
+  <si>
+    <t>Jesteśmy piękni</t>
+  </si>
+  <si>
+    <t>Jesteśmy piękni
+Twoim pięknem Panie!=
+Ty otwierasz nasze oczy,
+na piękno Twoje Panie!
+Ty otwierasz nasze oczy, Panie!
+Ty otwierasz nasze oczy
+na piękno Twoje Panie!
+Ty otwierasz nasze oczy, Panie, na Twoje piękno.</t>
+  </si>
+  <si>
+    <t>Ofiaruję Tobie</t>
+  </si>
+  <si>
+    <t>Ofiaruję Tobie, Panie mój
+Całe życie me
+Cały jestem Twój
+Aż na wieki
+Oto moje serce, przecież wiesz
+Tyś miłością mą
+Jedyną jest</t>
+  </si>
+  <si>
+    <t>Gdy się łączą ręce dwie</t>
+  </si>
+  <si>
+    <t>1.
+Gdy się łączą ręce dwie w Imię Boże,
+Przed ołtarzem uroczystym w blasku świec.
+Wtedy zwykła ludzka miłość jest potęgą,
+Bo z miłością Jego wieczną splata się.
+2.
+Kiedy łączysz serca dwa w Imię swoje
+I związujesz między nimi mocną nić.
+Błogosławisz swoim dzieciom na wędrówkę,
+Pokazujesz, co to znaczy umieć żyć.
+3.
+Pójdą odtąd na radości i na smutki,
+Zawsze razem, przy nim – ona, przy niej – on
+Twoja łaska szlak im będzie wyznaczała
+I obroni od drapieżnych świata szpon.</t>
+  </si>
+  <si>
+    <t>1/1/1/1/0/0</t>
+  </si>
+  <si>
+    <t>Szczęśliwy, kogo</t>
+  </si>
+  <si>
+    <t>1.
+Szczęśliwy, kogo opatrzność Boska
+ma w swej opiece, niech się nie troska:
+w żadnym przypadku ten nie szkoduje,
+kogo opatrzność Boska piastuje.
+2.
+Nie tak miedziany mur jest bezpieczny,
+ani też diament tak długowieczny,
+jak kto przy Bogu łaskawym stoi,
+żadnych się nieszczęść niechaj nie boi.
+3.
+Niechaj się na mnie i świat oburzy,
+niechaj me serce w żalach zanurzy;
+gdy tylko spojrzy Niebieskie Oko,
+wyjdę z tej toni pewnie wysoko.
+4.
+Boże Wszechmocny, nadzieje w Tobie
+nasze składamy, niech w każdej dobie
+przy nas opatrzność Twoja zostanie,
+bo nic bez Ciebie nie poczniem, Panie.</t>
   </si>
 </sst>
 </file>
@@ -13497,7 +13599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA72C7D-2EFC-408F-B255-EAEC24F0A3D2}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="D6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -13764,13 +13866,13 @@
   <sheetPr>
     <tabColor theme="2"/>
   </sheetPr>
-  <dimension ref="A1:G203"/>
+  <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B149" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -15158,441 +15260,429 @@
     </row>
     <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>113</v>
+        <v>580</v>
       </c>
       <c r="B62">
-        <v>6</v>
-      </c>
-      <c r="C62" t="s">
-        <v>285</v>
-      </c>
-      <c r="D62">
-        <v>315</v>
+        <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F62" t="s">
-        <v>335</v>
+        <v>572</v>
       </c>
       <c r="G62" s="25" t="s">
-        <v>532</v>
+        <v>581</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D63">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E63" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F63" t="s">
-        <v>358</v>
+        <v>335</v>
       </c>
       <c r="G63" s="25" t="s">
-        <v>442</v>
+        <v>532</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>317</v>
+        <v>286</v>
       </c>
       <c r="D64">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E64" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F64" t="s">
-        <v>342</v>
+        <v>358</v>
       </c>
       <c r="G64" s="25" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D65">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="E65" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F65" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
       <c r="G65" s="25" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>196</v>
+        <v>34</v>
       </c>
       <c r="B66">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>338</v>
+        <v>298</v>
       </c>
       <c r="D66">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E66" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F66" t="s">
-        <v>341</v>
+        <v>359</v>
       </c>
       <c r="G66" s="25" t="s">
-        <v>551</v>
+        <v>444</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>243</v>
+        <v>196</v>
       </c>
       <c r="B67">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
         <v>338</v>
       </c>
       <c r="D67">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E67" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="F67" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="G67" s="25" t="s">
-        <v>533</v>
+        <v>551</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>93</v>
+        <v>243</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C68" t="s">
-        <v>295</v>
+        <v>338</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>338</v>
       </c>
       <c r="E68" t="s">
-        <v>297</v>
+        <v>177</v>
       </c>
       <c r="F68" t="s">
         <v>335</v>
       </c>
+      <c r="G68" s="25" t="s">
+        <v>533</v>
+      </c>
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="B69">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="D69">
-        <v>352</v>
+        <v>0</v>
       </c>
       <c r="E69" t="s">
-        <v>175</v>
+        <v>297</v>
       </c>
       <c r="F69" t="s">
-        <v>360</v>
-      </c>
-      <c r="G69" s="25" t="s">
-        <v>445</v>
+        <v>335</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="D70">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="E70" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F70" t="s">
-        <v>346</v>
+        <v>360</v>
       </c>
       <c r="G70" s="25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B71">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="D71">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="E71" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F71" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="G71" s="25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>154</v>
+        <v>37</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D72">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="E72" t="s">
         <v>179</v>
       </c>
       <c r="F72" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="G72" s="25" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>154</v>
       </c>
       <c r="B73">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>338</v>
+        <v>290</v>
       </c>
       <c r="D73">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="E73" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="F73" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G73" s="25" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>155</v>
+        <v>38</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>289</v>
+        <v>338</v>
       </c>
       <c r="D74">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="E74" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="F74" t="s">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="G74" s="25" t="s">
-        <v>564</v>
+        <v>449</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="B75">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D75">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="E75" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="F75" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="G75" s="25" t="s">
-        <v>450</v>
+        <v>564</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D76">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E76" t="s">
         <v>171</v>
       </c>
       <c r="F76" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="G76" s="25" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>128</v>
+        <v>40</v>
       </c>
       <c r="B77">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="D77">
-        <v>431</v>
+        <v>406</v>
       </c>
       <c r="E77" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F77" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="G77" s="25" t="s">
-        <v>552</v>
+        <v>451</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>156</v>
+        <v>576</v>
       </c>
       <c r="B78">
-        <v>1</v>
-      </c>
-      <c r="C78" t="s">
-        <v>289</v>
-      </c>
-      <c r="D78">
-        <v>432</v>
+        <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="F78" t="s">
-        <v>341</v>
+        <v>572</v>
       </c>
       <c r="G78" s="25" t="s">
-        <v>452</v>
+        <v>577</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="D79">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="E79" t="s">
         <v>177</v>
       </c>
       <c r="F79" t="s">
-        <v>341</v>
+        <v>362</v>
       </c>
       <c r="G79" s="25" t="s">
-        <v>453</v>
+        <v>552</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="B80">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>311</v>
+        <v>289</v>
       </c>
       <c r="D80">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="E80" t="s">
         <v>171</v>
       </c>
       <c r="F80" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
       <c r="G80" s="25" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>44</v>
+        <v>157</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -15601,44 +15691,44 @@
         <v>289</v>
       </c>
       <c r="D81">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="E81" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F81" t="s">
         <v>341</v>
       </c>
       <c r="G81" s="25" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="B82">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>285</v>
+        <v>311</v>
       </c>
       <c r="D82">
-        <v>457</v>
+        <v>443</v>
       </c>
       <c r="E82" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="F82" t="s">
-        <v>335</v>
+        <v>360</v>
       </c>
       <c r="G82" s="25" t="s">
-        <v>534</v>
+        <v>454</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -15647,7 +15737,7 @@
         <v>289</v>
       </c>
       <c r="D83">
-        <v>468</v>
+        <v>439</v>
       </c>
       <c r="E83" t="s">
         <v>172</v>
@@ -15656,334 +15746,328 @@
         <v>341</v>
       </c>
       <c r="G83" s="25" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>43</v>
+        <v>114</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D84">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="E84" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F84" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G84" s="25" t="s">
-        <v>457</v>
+        <v>534</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>190</v>
+        <v>42</v>
       </c>
       <c r="B85">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C85" t="s">
-        <v>338</v>
+        <v>289</v>
       </c>
       <c r="D85">
-        <v>1314</v>
+        <v>468</v>
       </c>
       <c r="E85" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F85" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="G85" s="25" t="s">
-        <v>517</v>
+        <v>456</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B86">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D86">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="E86" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="F86" t="s">
-        <v>354</v>
+        <v>341</v>
       </c>
       <c r="G86" s="25" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>46</v>
+        <v>190</v>
       </c>
       <c r="B87">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="D87">
-        <v>483</v>
+        <v>1314</v>
       </c>
       <c r="E87" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F87" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="G87" s="25" t="s">
-        <v>459</v>
+        <v>517</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="D88">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="E88" t="s">
         <v>173</v>
       </c>
       <c r="F88" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="G88" s="25" t="s">
-        <v>398</v>
+        <v>458</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>208</v>
+        <v>46</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C89" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="D89">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="E89" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F89" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G89" s="25" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="B90">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C90" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D90">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="E90" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F90" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="G90" s="25" t="s">
-        <v>461</v>
+        <v>398</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>48</v>
+        <v>208</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>289</v>
+        <v>338</v>
       </c>
       <c r="D91">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="E91" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F91" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
       <c r="G91" s="25" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>49</v>
+        <v>574</v>
       </c>
       <c r="B92">
-        <v>4</v>
-      </c>
-      <c r="C92" t="s">
-        <v>311</v>
-      </c>
-      <c r="D92">
-        <v>496</v>
+        <v>2</v>
       </c>
       <c r="E92" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="F92" t="s">
-        <v>343</v>
+        <v>572</v>
       </c>
       <c r="G92" s="25" t="s">
-        <v>463</v>
+        <v>575</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>286</v>
+        <v>311</v>
       </c>
       <c r="D93">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="E93" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F93" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="G93" s="25" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
       <c r="C94" t="s">
-        <v>319</v>
+        <v>289</v>
       </c>
       <c r="D94">
-        <v>508</v>
+        <v>495</v>
       </c>
       <c r="E94" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="F94" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="G94" s="25" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>129</v>
+        <v>49</v>
       </c>
       <c r="B95">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C95" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="D95">
-        <v>514</v>
+        <v>496</v>
       </c>
       <c r="E95" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F95" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="G95" s="25" t="s">
-        <v>553</v>
+        <v>463</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C96" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="D96">
-        <v>520</v>
+        <v>503</v>
       </c>
       <c r="E96" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F96" t="s">
-        <v>336</v>
+        <v>355</v>
       </c>
       <c r="G96" s="25" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>130</v>
+        <v>51</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C97" t="s">
-        <v>279</v>
+        <v>319</v>
       </c>
       <c r="D97">
-        <v>1331</v>
+        <v>508</v>
       </c>
       <c r="E97" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F97" t="s">
         <v>347</v>
       </c>
       <c r="G97" s="25" t="s">
-        <v>379</v>
+        <v>465</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B98">
         <v>7</v>
@@ -15992,99 +16076,99 @@
         <v>279</v>
       </c>
       <c r="D98">
-        <v>539</v>
+        <v>514</v>
       </c>
       <c r="E98" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F98" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G98" s="25" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="B99">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C99" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="D99">
-        <v>540</v>
+        <v>520</v>
       </c>
       <c r="E99" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F99" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G99" s="25" t="s">
-        <v>535</v>
+        <v>466</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="B100">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C100" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D100">
-        <v>556</v>
+        <v>1331</v>
       </c>
       <c r="E100" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F100" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="G100" s="25" t="s">
-        <v>467</v>
+        <v>379</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="B101">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C101" t="s">
-        <v>338</v>
+        <v>279</v>
       </c>
       <c r="D101">
-        <v>558</v>
+        <v>539</v>
       </c>
       <c r="E101" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F101" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="G101" s="25" t="s">
-        <v>468</v>
+        <v>554</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B102">
         <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="D102">
-        <v>580</v>
+        <v>540</v>
       </c>
       <c r="E102" t="s">
         <v>172</v>
@@ -16093,196 +16177,190 @@
         <v>335</v>
       </c>
       <c r="G102" s="25" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B103">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C103" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D103">
-        <v>594</v>
+        <v>556</v>
       </c>
       <c r="E103" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="F103" t="s">
         <v>342</v>
       </c>
       <c r="G103" s="25" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="B104">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C104" t="s">
-        <v>278</v>
+        <v>338</v>
       </c>
       <c r="D104">
-        <v>598</v>
+        <v>558</v>
       </c>
       <c r="E104" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="F104" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="G104" s="25" t="s">
-        <v>537</v>
+        <v>468</v>
       </c>
     </row>
     <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="B105">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C105" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D105">
-        <v>611</v>
+        <v>580</v>
       </c>
       <c r="E105" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F105" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="G105" s="25" t="s">
-        <v>470</v>
+        <v>536</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>57</v>
+        <v>571</v>
       </c>
       <c r="B106">
-        <v>4</v>
-      </c>
-      <c r="C106" t="s">
-        <v>311</v>
-      </c>
-      <c r="D106">
-        <v>623</v>
+        <v>2</v>
       </c>
       <c r="E106" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F106" t="s">
-        <v>347</v>
+        <v>572</v>
       </c>
       <c r="G106" s="25" t="s">
-        <v>471</v>
+        <v>573</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>274</v>
+        <v>55</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
       <c r="C107" t="s">
-        <v>338</v>
+        <v>289</v>
       </c>
       <c r="D107">
-        <v>630</v>
+        <v>594</v>
       </c>
       <c r="E107" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F107" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="G107" s="25" t="s">
-        <v>326</v>
+        <v>469</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>158</v>
+        <v>117</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C108" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D108">
-        <v>631</v>
+        <v>598</v>
       </c>
       <c r="E108" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F108" t="s">
-        <v>363</v>
+        <v>335</v>
       </c>
       <c r="G108" s="25" t="s">
-        <v>472</v>
+        <v>537</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>244</v>
+        <v>56</v>
       </c>
       <c r="B109">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>338</v>
+        <v>288</v>
       </c>
       <c r="D109">
-        <v>640</v>
+        <v>611</v>
       </c>
       <c r="E109" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F109" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="G109" s="25" t="s">
-        <v>538</v>
+        <v>470</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>210</v>
+        <v>57</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C110" t="s">
-        <v>338</v>
+        <v>311</v>
       </c>
       <c r="D110">
-        <v>641</v>
+        <v>623</v>
       </c>
       <c r="E110" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F110" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="G110" s="25" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -16291,87 +16369,90 @@
         <v>338</v>
       </c>
       <c r="D111">
-        <v>647</v>
+        <v>630</v>
       </c>
       <c r="E111" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F111" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="G111" s="25" t="s">
-        <v>474</v>
+        <v>326</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>60</v>
+        <v>158</v>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C112" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D112">
-        <v>649</v>
+        <v>631</v>
       </c>
       <c r="E112" t="s">
         <v>182</v>
       </c>
       <c r="F112" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
       <c r="G112" s="25" t="s">
-        <v>400</v>
+        <v>472</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>138</v>
+        <v>244</v>
       </c>
       <c r="B113">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C113" t="s">
-        <v>312</v>
+        <v>338</v>
       </c>
       <c r="D113">
-        <v>655</v>
+        <v>640</v>
       </c>
       <c r="E113" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="F113" t="s">
-        <v>342</v>
+        <v>335</v>
+      </c>
+      <c r="G113" s="25" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>58</v>
+        <v>210</v>
       </c>
       <c r="B114">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C114" t="s">
-        <v>282</v>
+        <v>338</v>
       </c>
       <c r="D114">
-        <v>656</v>
+        <v>641</v>
       </c>
       <c r="E114" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F114" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="G114" s="25" t="s">
-        <v>518</v>
+        <v>473</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -16380,725 +16461,722 @@
         <v>338</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>647</v>
       </c>
       <c r="E115" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="F115" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G115" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
       <c r="B116">
         <v>2</v>
       </c>
       <c r="C116" t="s">
-        <v>313</v>
+        <v>288</v>
       </c>
       <c r="D116">
-        <v>672</v>
+        <v>649</v>
       </c>
       <c r="E116" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="F116" t="s">
-        <v>364</v>
+        <v>347</v>
+      </c>
+      <c r="G116" s="25" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>381</v>
+        <v>138</v>
       </c>
       <c r="B117">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C117" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="D117">
-        <v>1308</v>
+        <v>655</v>
       </c>
       <c r="E117" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F117" t="s">
-        <v>335</v>
-      </c>
-      <c r="G117" s="25" t="s">
-        <v>382</v>
+        <v>342</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B118">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="D118">
-        <v>677</v>
+        <v>656</v>
       </c>
       <c r="E118" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F118" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="G118" s="25" t="s">
-        <v>475</v>
+        <v>518</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>262</v>
       </c>
       <c r="B119">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C119" t="s">
-        <v>278</v>
+        <v>338</v>
       </c>
       <c r="D119">
-        <v>687</v>
+        <v>0</v>
       </c>
       <c r="E119" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F119" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="G119" s="25" t="s">
-        <v>539</v>
+        <v>476</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>61</v>
+        <v>137</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C120" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D120">
-        <v>690</v>
+        <v>672</v>
       </c>
       <c r="E120" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F120" t="s">
-        <v>365</v>
-      </c>
-      <c r="G120" s="25" t="s">
-        <v>477</v>
+        <v>364</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>240</v>
+        <v>381</v>
       </c>
       <c r="B121">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C121" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="D121">
-        <v>700</v>
+        <v>1308</v>
       </c>
       <c r="E121" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F121" t="s">
         <v>335</v>
       </c>
       <c r="G121" s="25" t="s">
-        <v>540</v>
+        <v>382</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="B122">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C122" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="D122">
-        <v>709</v>
+        <v>677</v>
       </c>
       <c r="E122" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="F122" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="G122" s="25" t="s">
-        <v>555</v>
+        <v>475</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C123" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="D123">
-        <v>726</v>
+        <v>687</v>
       </c>
       <c r="E123" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F123" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G123" s="25" t="s">
-        <v>478</v>
+        <v>539</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B124">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C124" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="D124">
-        <v>727</v>
+        <v>690</v>
       </c>
       <c r="E124" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="F124" t="s">
-        <v>341</v>
+        <v>365</v>
       </c>
       <c r="G124" s="25" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>64</v>
+        <v>240</v>
       </c>
       <c r="B125">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C125" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="D125">
-        <v>732</v>
+        <v>700</v>
       </c>
       <c r="E125" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="F125" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="G125" s="25" t="s">
-        <v>480</v>
+        <v>540</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>15</v>
+        <v>159</v>
       </c>
       <c r="B126">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C126" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="D126">
-        <v>733</v>
+        <v>709</v>
       </c>
       <c r="E126" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F126" t="s">
-        <v>366</v>
+        <v>341</v>
       </c>
       <c r="G126" s="25" t="s">
-        <v>481</v>
+        <v>555</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="B127">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C127" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="D127">
-        <v>745</v>
+        <v>726</v>
       </c>
       <c r="E127" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F127" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="G127" s="25" t="s">
-        <v>333</v>
+        <v>478</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>132</v>
+        <v>63</v>
       </c>
       <c r="B128">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C128" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="D128">
-        <v>771</v>
+        <v>727</v>
       </c>
       <c r="E128" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F128" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="G128" s="25" t="s">
-        <v>556</v>
+        <v>479</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B129">
         <v>1</v>
       </c>
       <c r="C129" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D129">
-        <v>778</v>
+        <v>732</v>
       </c>
       <c r="E129" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F129" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="G129" s="25" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>103</v>
+        <v>15</v>
       </c>
       <c r="B130">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C130" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
       <c r="D130">
-        <v>789</v>
+        <v>733</v>
       </c>
       <c r="E130" t="s">
         <v>173</v>
       </c>
       <c r="F130" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="G130" s="25" t="s">
-        <v>519</v>
+        <v>481</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>204</v>
+        <v>95</v>
       </c>
       <c r="B131">
         <v>2</v>
       </c>
       <c r="C131" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D131">
-        <v>796</v>
+        <v>745</v>
       </c>
       <c r="E131" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F131" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="G131" s="25" t="s">
-        <v>401</v>
+        <v>333</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>139</v>
+        <v>578</v>
       </c>
       <c r="B132">
-        <v>8</v>
-      </c>
-      <c r="C132" t="s">
-        <v>312</v>
+        <v>1</v>
       </c>
       <c r="D132">
-        <v>797</v>
+        <v>769</v>
       </c>
       <c r="E132" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F132" t="s">
-        <v>341</v>
+        <v>342</v>
+      </c>
+      <c r="G132" s="25" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>236</v>
+        <v>132</v>
       </c>
       <c r="B133">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C133" t="s">
-        <v>338</v>
+        <v>279</v>
       </c>
       <c r="D133">
-        <v>806</v>
+        <v>771</v>
       </c>
       <c r="E133" t="s">
         <v>177</v>
       </c>
       <c r="F133" t="s">
-        <v>342</v>
+        <v>355</v>
       </c>
       <c r="G133" s="25" t="s">
-        <v>483</v>
+        <v>556</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B134">
         <v>1</v>
       </c>
       <c r="C134" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="D134">
-        <v>812</v>
+        <v>778</v>
       </c>
       <c r="E134" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F134" t="s">
         <v>341</v>
       </c>
       <c r="G134" s="25" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D135">
-        <v>819</v>
+        <v>789</v>
       </c>
       <c r="E135" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F135" t="s">
-        <v>341</v>
+        <v>367</v>
       </c>
       <c r="G135" s="25" t="s">
-        <v>485</v>
+        <v>519</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>246</v>
+        <v>204</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C136" t="s">
-        <v>289</v>
+        <v>302</v>
       </c>
       <c r="D136">
-        <v>823</v>
+        <v>796</v>
       </c>
       <c r="E136" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F136" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="G136" s="25" t="s">
-        <v>486</v>
+        <v>401</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>139</v>
       </c>
       <c r="B137">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C137" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="D137">
-        <v>835</v>
+        <v>797</v>
       </c>
       <c r="E137" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F137" t="s">
-        <v>360</v>
-      </c>
-      <c r="G137" s="25" t="s">
-        <v>487</v>
+        <v>341</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>67</v>
+        <v>236</v>
       </c>
       <c r="B138">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C138" t="s">
-        <v>286</v>
+        <v>338</v>
       </c>
       <c r="D138">
-        <v>856</v>
+        <v>806</v>
       </c>
       <c r="E138" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F138" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="G138" s="25" t="s">
-        <v>402</v>
+        <v>483</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B139">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C139" t="s">
-        <v>338</v>
+        <v>289</v>
       </c>
       <c r="D139">
-        <v>861</v>
+        <v>812</v>
       </c>
       <c r="E139" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="F139" t="s">
-        <v>355</v>
+        <v>341</v>
       </c>
       <c r="G139" s="25" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>237</v>
+        <v>66</v>
       </c>
       <c r="B140">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C140" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="D140">
-        <v>862</v>
+        <v>819</v>
       </c>
       <c r="E140" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F140" t="s">
-        <v>368</v>
+        <v>341</v>
       </c>
       <c r="G140" s="25" t="s">
-        <v>520</v>
+        <v>485</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>68</v>
+        <v>246</v>
       </c>
       <c r="B141">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C141" t="s">
-        <v>311</v>
+        <v>289</v>
       </c>
       <c r="D141">
-        <v>863</v>
+        <v>823</v>
       </c>
       <c r="E141" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F141" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="G141" s="25" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B142">
         <v>1</v>
       </c>
       <c r="C142" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D142">
-        <v>870</v>
+        <v>835</v>
       </c>
       <c r="E142" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F142" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="G142" s="25" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>380</v>
+        <v>67</v>
       </c>
       <c r="B143">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C143" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="D143">
-        <v>1308</v>
+        <v>856</v>
       </c>
       <c r="E143" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F143" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G143" s="25" t="s">
-        <v>383</v>
+        <v>402</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>334</v>
+        <v>69</v>
       </c>
       <c r="B144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C144" t="s">
-        <v>295</v>
+        <v>338</v>
+      </c>
+      <c r="D144">
+        <v>861</v>
       </c>
       <c r="E144" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F144" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="G144" s="25" t="s">
-        <v>375</v>
+        <v>488</v>
       </c>
     </row>
     <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>201</v>
+        <v>237</v>
       </c>
       <c r="B145">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C145" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D145">
-        <v>899</v>
+        <v>862</v>
       </c>
       <c r="E145" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F145" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G145" s="25" t="s">
-        <v>557</v>
+        <v>520</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B146">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C146" t="s">
-        <v>298</v>
+        <v>311</v>
       </c>
       <c r="D146">
-        <v>876</v>
+        <v>863</v>
       </c>
       <c r="E146" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F146" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G146" s="25" t="s">
-        <v>329</v>
+        <v>489</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>161</v>
+        <v>13</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -17107,44 +17185,44 @@
         <v>298</v>
       </c>
       <c r="D147">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="E147" t="s">
         <v>172</v>
       </c>
       <c r="F147" t="s">
-        <v>336</v>
+        <v>352</v>
       </c>
       <c r="G147" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="148" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>119</v>
+        <v>380</v>
       </c>
       <c r="B148">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C148" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="D148">
-        <v>879</v>
+        <v>1308</v>
       </c>
       <c r="E148" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F148" t="s">
         <v>335</v>
       </c>
       <c r="G148" s="25" t="s">
-        <v>541</v>
+        <v>383</v>
       </c>
     </row>
     <row r="149" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>96</v>
+        <v>334</v>
       </c>
       <c r="B149">
         <v>2</v>
@@ -17152,298 +17230,295 @@
       <c r="C149" t="s">
         <v>295</v>
       </c>
-      <c r="D149">
-        <v>920</v>
-      </c>
       <c r="E149" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F149" t="s">
-        <v>335</v>
+        <v>374</v>
       </c>
       <c r="G149" s="25" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>97</v>
+        <v>201</v>
       </c>
       <c r="B150">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C150" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="D150">
-        <v>934</v>
+        <v>899</v>
       </c>
       <c r="E150" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F150" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="G150" s="25" t="s">
-        <v>403</v>
+        <v>557</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="B151">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C151" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D151">
-        <v>938</v>
+        <v>876</v>
       </c>
       <c r="E151" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F151" t="s">
-        <v>335</v>
+        <v>349</v>
       </c>
       <c r="G151" s="25" t="s">
-        <v>542</v>
+        <v>329</v>
       </c>
     </row>
     <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="B152">
         <v>1</v>
       </c>
       <c r="C152" t="s">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="D152">
-        <v>940</v>
+        <v>878</v>
       </c>
       <c r="E152" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F152" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G152" s="25" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>193</v>
+        <v>119</v>
       </c>
       <c r="B153">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="D153">
-        <v>951</v>
+        <v>879</v>
       </c>
       <c r="E153" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F153" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G153" s="25" t="s">
-        <v>328</v>
+        <v>541</v>
       </c>
     </row>
     <row r="154" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C154" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="D154">
-        <v>954</v>
+        <v>920</v>
       </c>
       <c r="E154" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F154" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="G154" s="25" t="s">
-        <v>493</v>
+        <v>384</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C155" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="D155">
-        <v>973</v>
+        <v>934</v>
       </c>
       <c r="E155" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F155" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="G155" s="25" t="s">
-        <v>494</v>
+        <v>403</v>
       </c>
     </row>
     <row r="156" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="B156">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C156" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D156">
-        <v>985</v>
+        <v>938</v>
       </c>
       <c r="E156" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F156" t="s">
-        <v>349</v>
+        <v>335</v>
       </c>
       <c r="G156" s="25" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>265</v>
+        <v>71</v>
       </c>
       <c r="B157">
         <v>1</v>
       </c>
       <c r="C157" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="D157">
-        <v>990</v>
+        <v>940</v>
       </c>
       <c r="E157" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F157" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="G157" s="25" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B158">
         <v>1</v>
       </c>
       <c r="C158" t="s">
-        <v>338</v>
+        <v>298</v>
       </c>
       <c r="D158">
-        <v>1295</v>
+        <v>951</v>
       </c>
       <c r="E158" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="F158" t="s">
         <v>341</v>
       </c>
       <c r="G158" s="25" t="s">
-        <v>496</v>
+        <v>328</v>
       </c>
     </row>
     <row r="159" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B159">
         <v>1</v>
       </c>
       <c r="C159" t="s">
-        <v>279</v>
+        <v>317</v>
       </c>
       <c r="D159">
-        <v>999</v>
+        <v>954</v>
       </c>
       <c r="E159" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="F159" t="s">
         <v>342</v>
       </c>
       <c r="G159" s="25" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="160" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B160">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C160" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D160">
-        <v>1002</v>
+        <v>973</v>
       </c>
       <c r="E160" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F160" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="G160" s="25" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="B161">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C161" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D161">
-        <v>1005</v>
+        <v>985</v>
       </c>
       <c r="E161" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F161" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="G161" s="25" t="s">
-        <v>499</v>
+        <v>558</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>164</v>
+        <v>265</v>
       </c>
       <c r="B162">
         <v>1</v>
@@ -17452,656 +17527,656 @@
         <v>289</v>
       </c>
       <c r="D162">
-        <v>1009</v>
+        <v>990</v>
       </c>
       <c r="E162" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F162" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="G162" s="25" t="s">
-        <v>331</v>
+        <v>495</v>
       </c>
     </row>
     <row r="163" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="B163">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C163" t="s">
-        <v>303</v>
+        <v>338</v>
       </c>
       <c r="D163">
-        <v>1333</v>
+        <v>1295</v>
       </c>
       <c r="E163" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F163" t="s">
-        <v>370</v>
+        <v>341</v>
       </c>
       <c r="G163" s="25" t="s">
-        <v>404</v>
+        <v>496</v>
       </c>
     </row>
     <row r="164" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="B164">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C164" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D164">
-        <v>1027</v>
+        <v>999</v>
       </c>
       <c r="E164" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="F164" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="G164" s="25" t="s">
-        <v>521</v>
+        <v>497</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>305</v>
+        <v>74</v>
       </c>
       <c r="B165">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C165" t="s">
-        <v>293</v>
-      </c>
-      <c r="D165" t="s">
-        <v>406</v>
+        <v>311</v>
+      </c>
+      <c r="D165">
+        <v>1002</v>
       </c>
       <c r="E165" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F165" t="s">
         <v>347</v>
       </c>
       <c r="G165" s="25" t="s">
-        <v>405</v>
+        <v>498</v>
       </c>
     </row>
     <row r="166" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="B166">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C166" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="D166">
-        <v>1047</v>
+        <v>1005</v>
       </c>
       <c r="E166" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F166" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="G166" s="25" t="s">
-        <v>387</v>
+        <v>499</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="B167">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C167" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="D167">
-        <v>1067</v>
+        <v>1009</v>
       </c>
       <c r="E167" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="F167" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="G167" s="25" t="s">
-        <v>543</v>
+        <v>331</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B168">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C168" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D168">
-        <v>1069</v>
+        <v>1333</v>
       </c>
       <c r="E168" t="s">
-        <v>263</v>
+        <v>176</v>
       </c>
       <c r="F168" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="G168" s="25" t="s">
-        <v>500</v>
+        <v>404</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="B169">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C169" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D169">
-        <v>1070</v>
+        <v>1027</v>
       </c>
       <c r="E169" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F169" t="s">
-        <v>371</v>
+        <v>337</v>
       </c>
       <c r="G169" s="25" t="s">
-        <v>407</v>
+        <v>521</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>79</v>
+        <v>583</v>
       </c>
       <c r="B170">
         <v>1</v>
       </c>
       <c r="C170" t="s">
-        <v>289</v>
-      </c>
-      <c r="D170">
-        <v>1086</v>
+        <v>298</v>
       </c>
       <c r="E170" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="F170" t="s">
-        <v>341</v>
+        <v>362</v>
       </c>
       <c r="G170" s="25" t="s">
-        <v>501</v>
+        <v>584</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>186</v>
+        <v>305</v>
       </c>
       <c r="B171">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C171" t="s">
-        <v>338</v>
-      </c>
-      <c r="D171">
-        <v>1283</v>
+        <v>293</v>
+      </c>
+      <c r="D171" t="s">
+        <v>406</v>
       </c>
       <c r="E171" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F171" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G171" s="25" t="s">
-        <v>502</v>
+        <v>405</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="B172">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C172" t="s">
-        <v>317</v>
+        <v>295</v>
       </c>
       <c r="D172">
-        <v>1095</v>
+        <v>1047</v>
       </c>
       <c r="E172" t="s">
         <v>182</v>
       </c>
       <c r="F172" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="G172" s="25" t="s">
-        <v>503</v>
+        <v>387</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="B173">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C173" t="s">
-        <v>307</v>
+        <v>278</v>
       </c>
       <c r="D173">
-        <v>1100</v>
+        <v>1067</v>
       </c>
       <c r="E173" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F173" t="s">
-        <v>408</v>
+        <v>335</v>
       </c>
       <c r="G173" s="25" t="s">
-        <v>409</v>
+        <v>543</v>
       </c>
     </row>
     <row r="174" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="B174">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C174" t="s">
-        <v>285</v>
+        <v>311</v>
       </c>
       <c r="D174">
-        <v>1114</v>
+        <v>1069</v>
       </c>
       <c r="E174" t="s">
-        <v>173</v>
+        <v>263</v>
       </c>
       <c r="F174" t="s">
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="G174" s="25" t="s">
-        <v>544</v>
+        <v>500</v>
       </c>
     </row>
     <row r="175" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="B175">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C175" t="s">
-        <v>338</v>
+        <v>289</v>
       </c>
       <c r="D175">
-        <v>1120</v>
+        <v>1070</v>
       </c>
       <c r="E175" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F175" t="s">
-        <v>347</v>
+        <v>371</v>
       </c>
       <c r="G175" s="25" t="s">
-        <v>559</v>
+        <v>407</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="B176">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C176" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="D176">
-        <v>1130</v>
+        <v>1086</v>
       </c>
       <c r="E176" t="s">
         <v>173</v>
       </c>
       <c r="F176" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="G176" s="25" t="s">
-        <v>545</v>
+        <v>501</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>140</v>
+        <v>186</v>
       </c>
       <c r="B177">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C177" t="s">
-        <v>312</v>
+        <v>338</v>
       </c>
       <c r="D177">
-        <v>1135</v>
+        <v>1283</v>
       </c>
       <c r="E177" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="F177" t="s">
-        <v>347</v>
+        <v>349</v>
+      </c>
+      <c r="G177" s="25" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="B178">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C178" t="s">
-        <v>278</v>
+        <v>317</v>
       </c>
       <c r="D178">
-        <v>1139</v>
+        <v>1095</v>
       </c>
       <c r="E178" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="F178" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="G178" s="25" t="s">
-        <v>546</v>
+        <v>503</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>141</v>
+        <v>80</v>
       </c>
       <c r="B179">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C179" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D179">
-        <v>1140</v>
+        <v>1100</v>
       </c>
       <c r="E179" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F179" t="s">
-        <v>372</v>
+        <v>408</v>
+      </c>
+      <c r="G179" s="25" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="B180">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C180" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D180">
-        <v>1151</v>
+        <v>1114</v>
       </c>
       <c r="E180" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F180" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="G180" s="25" t="s">
-        <v>504</v>
+        <v>544</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B181">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C181" t="s">
-        <v>279</v>
+        <v>338</v>
       </c>
       <c r="D181">
-        <v>1165</v>
+        <v>1120</v>
       </c>
       <c r="E181" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F181" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="G181" s="25" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="182" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>205</v>
+        <v>125</v>
       </c>
       <c r="B182">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C182" t="s">
-        <v>338</v>
+        <v>278</v>
       </c>
       <c r="D182">
-        <v>1168</v>
+        <v>1130</v>
       </c>
       <c r="E182" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F182" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G182" s="25" t="s">
-        <v>505</v>
+        <v>545</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="B183">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C183" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D183">
-        <v>0</v>
+        <v>1135</v>
       </c>
       <c r="E183" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F183" t="s">
-        <v>341</v>
-      </c>
-      <c r="G183" s="25" t="s">
-        <v>423</v>
+        <v>347</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>82</v>
+        <v>123</v>
       </c>
       <c r="B184">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="D184">
-        <v>1176</v>
+        <v>1139</v>
       </c>
       <c r="E184" t="s">
         <v>173</v>
       </c>
       <c r="F184" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
       <c r="G184" s="25" t="s">
-        <v>410</v>
+        <v>546</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="B185">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C185" t="s">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c r="D185">
-        <v>1184</v>
+        <v>1140</v>
       </c>
       <c r="E185" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F185" t="s">
-        <v>336</v>
-      </c>
-      <c r="G185" s="25" t="s">
-        <v>506</v>
+        <v>372</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>271</v>
+        <v>81</v>
       </c>
       <c r="B186">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C186" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="D186">
-        <v>0</v>
+        <v>1151</v>
       </c>
       <c r="E186" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F186" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="G186" s="25" t="s">
-        <v>561</v>
+        <v>504</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>272</v>
+        <v>134</v>
       </c>
       <c r="B187">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C187" t="s">
-        <v>312</v>
+        <v>279</v>
       </c>
       <c r="D187">
-        <v>1196</v>
+        <v>1165</v>
       </c>
       <c r="E187" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="F187" t="s">
-        <v>342</v>
+        <v>341</v>
+      </c>
+      <c r="G187" s="25" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>84</v>
+        <v>205</v>
       </c>
       <c r="B188">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C188" t="s">
-        <v>298</v>
+        <v>338</v>
       </c>
       <c r="D188">
-        <v>1203</v>
+        <v>1168</v>
       </c>
       <c r="E188" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F188" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="G188" s="25" t="s">
-        <v>399</v>
+        <v>505</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="B189">
         <v>1</v>
       </c>
       <c r="C189" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="D189">
-        <v>1205</v>
+        <v>0</v>
       </c>
       <c r="E189" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F189" t="s">
-        <v>359</v>
+        <v>341</v>
       </c>
       <c r="G189" s="25" t="s">
-        <v>507</v>
+        <v>423</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>124</v>
+        <v>82</v>
       </c>
       <c r="B190">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C190" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="D190">
-        <v>1194</v>
+        <v>1176</v>
       </c>
       <c r="E190" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F190" t="s">
-        <v>335</v>
+        <v>356</v>
       </c>
       <c r="G190" s="25" t="s">
-        <v>547</v>
+        <v>410</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B191">
         <v>3</v>
@@ -18110,293 +18185,428 @@
         <v>286</v>
       </c>
       <c r="D191">
-        <v>1223</v>
+        <v>1184</v>
       </c>
       <c r="E191" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F191" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="G191" s="25" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>126</v>
+        <v>271</v>
       </c>
       <c r="B192">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C192" t="s">
-        <v>278</v>
+        <v>309</v>
       </c>
       <c r="D192">
-        <v>1224</v>
+        <v>0</v>
       </c>
       <c r="E192" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F192" t="s">
-        <v>335</v>
+        <v>373</v>
       </c>
       <c r="G192" s="25" t="s">
-        <v>548</v>
+        <v>561</v>
       </c>
     </row>
     <row r="193" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>169</v>
+        <v>272</v>
       </c>
       <c r="B193">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C193" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="D193">
-        <v>1226</v>
+        <v>1196</v>
       </c>
       <c r="E193" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F193" t="s">
         <v>342</v>
       </c>
-      <c r="G193" s="25" t="s">
-        <v>422</v>
-      </c>
     </row>
     <row r="194" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>167</v>
+        <v>84</v>
       </c>
       <c r="B194">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C194" t="s">
         <v>298</v>
       </c>
       <c r="D194">
-        <v>1237</v>
+        <v>1203</v>
       </c>
       <c r="E194" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F194" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="G194" s="25" t="s">
-        <v>509</v>
+        <v>399</v>
       </c>
     </row>
     <row r="195" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>192</v>
+        <v>9</v>
       </c>
       <c r="B195">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C195" t="s">
-        <v>338</v>
+        <v>298</v>
       </c>
       <c r="D195">
-        <v>845</v>
+        <v>1205</v>
       </c>
       <c r="E195" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="F195" t="s">
-        <v>347</v>
+        <v>582</v>
       </c>
       <c r="G195" s="25" t="s">
-        <v>411</v>
+        <v>507</v>
       </c>
     </row>
     <row r="196" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B196">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C196" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D196">
-        <v>1245</v>
+        <v>1194</v>
       </c>
       <c r="E196" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="F196" t="s">
         <v>335</v>
       </c>
       <c r="G196" s="25" t="s">
-        <v>385</v>
+        <v>547</v>
       </c>
     </row>
     <row r="197" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B197">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C197" t="s">
         <v>286</v>
       </c>
       <c r="D197">
-        <v>1248</v>
+        <v>1223</v>
       </c>
       <c r="E197" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F197" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="G197" s="25" t="s">
-        <v>386</v>
+        <v>508</v>
       </c>
     </row>
     <row r="198" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="B198">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C198" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="D198">
-        <v>1252</v>
+        <v>1224</v>
       </c>
       <c r="E198" t="s">
         <v>175</v>
       </c>
       <c r="F198" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G198" s="25" t="s">
-        <v>510</v>
+        <v>548</v>
       </c>
     </row>
     <row r="199" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="B199">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C199" t="s">
-        <v>282</v>
+        <v>317</v>
       </c>
       <c r="D199">
-        <v>1253</v>
+        <v>1226</v>
       </c>
       <c r="E199" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F199" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="G199" s="25" t="s">
-        <v>522</v>
+        <v>422</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>12</v>
+        <v>167</v>
       </c>
       <c r="B200">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C200" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="D200">
-        <v>1255</v>
+        <v>1237</v>
       </c>
       <c r="E200" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F200" t="s">
         <v>342</v>
       </c>
       <c r="G200" s="25" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="B201">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C201" t="s">
-        <v>298</v>
+        <v>338</v>
       </c>
       <c r="D201">
-        <v>1262</v>
+        <v>845</v>
       </c>
       <c r="E201" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F201" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="G201" s="25" t="s">
-        <v>512</v>
+        <v>411</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="B202">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C202" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D202">
-        <v>1276</v>
+        <v>1245</v>
       </c>
       <c r="E202" t="s">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c r="F202" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G202" s="25" t="s">
-        <v>513</v>
+        <v>385</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>101</v>
+      </c>
+      <c r="B203">
+        <v>2</v>
+      </c>
+      <c r="C203" t="s">
+        <v>286</v>
+      </c>
+      <c r="D203">
+        <v>1248</v>
+      </c>
+      <c r="E203" t="s">
+        <v>175</v>
+      </c>
+      <c r="F203" t="s">
+        <v>335</v>
+      </c>
+      <c r="G203" s="25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>85</v>
+      </c>
+      <c r="B204">
+        <v>1</v>
+      </c>
+      <c r="C204" t="s">
+        <v>289</v>
+      </c>
+      <c r="D204">
+        <v>1252</v>
+      </c>
+      <c r="E204" t="s">
+        <v>175</v>
+      </c>
+      <c r="F204" t="s">
+        <v>341</v>
+      </c>
+      <c r="G204" s="25" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>87</v>
+      </c>
+      <c r="B205">
+        <v>5</v>
+      </c>
+      <c r="C205" t="s">
+        <v>282</v>
+      </c>
+      <c r="D205">
+        <v>1253</v>
+      </c>
+      <c r="E205" t="s">
+        <v>175</v>
+      </c>
+      <c r="F205" t="s">
+        <v>337</v>
+      </c>
+      <c r="G205" s="25" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>12</v>
+      </c>
+      <c r="B206">
+        <v>3</v>
+      </c>
+      <c r="C206" t="s">
+        <v>286</v>
+      </c>
+      <c r="D206">
+        <v>1255</v>
+      </c>
+      <c r="E206" t="s">
+        <v>179</v>
+      </c>
+      <c r="F206" t="s">
+        <v>342</v>
+      </c>
+      <c r="G206" s="25" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>168</v>
+      </c>
+      <c r="B207">
+        <v>1</v>
+      </c>
+      <c r="C207" t="s">
+        <v>298</v>
+      </c>
+      <c r="D207">
+        <v>1262</v>
+      </c>
+      <c r="E207" t="s">
+        <v>171</v>
+      </c>
+      <c r="F207" t="s">
+        <v>343</v>
+      </c>
+      <c r="G207" s="25" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>170</v>
+      </c>
+      <c r="B208">
+        <v>1</v>
+      </c>
+      <c r="C208" t="s">
+        <v>289</v>
+      </c>
+      <c r="D208">
+        <v>1276</v>
+      </c>
+      <c r="E208" t="s">
+        <v>176</v>
+      </c>
+      <c r="F208" t="s">
+        <v>341</v>
+      </c>
+      <c r="G208" s="25" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>142</v>
       </c>
-      <c r="B203">
+      <c r="B209">
         <v>8</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C209" t="s">
         <v>312</v>
       </c>
-      <c r="D203">
+      <c r="D209">
         <v>1279</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E209" t="s">
         <v>171</v>
       </c>
-      <c r="F203" t="s">
+      <c r="F209" t="s">
         <v>339</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G203" xr:uid="{4F891C4F-9816-403C-B080-E89BC2162DC9}"/>
+  <autoFilter ref="A1:G209" xr:uid="{4F891C4F-9816-403C-B080-E89BC2162DC9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>